<commit_message>
note of instruction added
</commit_message>
<xml_diff>
--- a/function.xlsx
+++ b/function.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Purdue\3\30862\PC++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4E6FA5-8CF7-47FB-93FF-88287E17A57F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEEA6B2-9951-4BC4-AEB4-977869B92F86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7F89506E-479F-4ED2-B304-C655C4E248C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>load file to memory</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +166,14 @@
   </si>
   <si>
     <t>interpreter.cpp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intepreter class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instruction enum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -683,229 +691,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03836210-BD8A-44FA-9EDA-D3FE262B3917}">
-  <dimension ref="A4:Q17"/>
+  <dimension ref="A4:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="51.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" style="10" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:17" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="2" t="s">
+    <row r="4" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="2" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="2" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="11"/>
-    </row>
-    <row r="6" spans="1:17" s="8" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="I6" s="9" t="s">
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="J6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="H8" s="3" t="s">
+    <row r="7" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="2" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="11"/>
-    </row>
-    <row r="9" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="I9" s="1" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="5" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="5" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="I10" s="1" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="I11" s="1" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="10"/>
-    </row>
-    <row r="12" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="I12" s="1" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="10"/>
-    </row>
-    <row r="13" spans="1:17" s="8" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="I13" s="9" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" s="8" customFormat="1" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="12"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="H14" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J15" s="5" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J16" s="5" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="14:16" x14ac:dyDescent="0.3">
-      <c r="N17" s="5" t="s">
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>